<commit_message>
Merged Beef and Lamb and modified food groups labels in script and dalys_values excel file
</commit_message>
<xml_diff>
--- a/data/XLSX/dalys_values.xlsx
+++ b/data/XLSX/dalys_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/luc_warde_fao_org/Documents/Document/Shinyapp/esf-shiny-DALYs/data/XLSX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfao-my.sharepoint.com/personal/stefano_dicandia_fao_org/Documents/Documenti/esf-shiny-DALYs/data/XLSX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{3EE426F9-AC1B-4E4D-B5CF-ECC4F6DF080F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFAE3F0A-B36C-7745-9FD1-26C6893BBB27}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{3EE426F9-AC1B-4E4D-B5CF-ECC4F6DF080F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9A38E8C-0835-4955-B988-4E5DA3FA24C9}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="900" windowWidth="28040" windowHeight="17180" xr2:uid="{E7303344-5A6B-444A-8B50-38B689E7ED8E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E7303344-5A6B-444A-8B50-38B689E7ED8E}"/>
   </bookViews>
   <sheets>
     <sheet name="dalys_values" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t>country</t>
   </si>
@@ -43,24 +43,12 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>Lamb</t>
-  </si>
-  <si>
-    <t>Beef</t>
-  </si>
-  <si>
     <t>Pork</t>
   </si>
   <si>
-    <t>Poultry</t>
-  </si>
-  <si>
     <t>Eggs</t>
   </si>
   <si>
-    <t>Dairy</t>
-  </si>
-  <si>
     <t>Fish and shellfish</t>
   </si>
   <si>
@@ -70,13 +58,22 @@
     <t>Beverages</t>
   </si>
   <si>
-    <t>Grains,bread, pastas and bakery products</t>
-  </si>
-  <si>
     <t>Other foods including composite foods</t>
   </si>
   <si>
     <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Beef and lamb</t>
+  </si>
+  <si>
+    <t>Chicken and other poultry</t>
+  </si>
+  <si>
+    <t>Dairy products</t>
+  </si>
+  <si>
+    <t>Bread, grains, pastas, and bakery products</t>
   </si>
 </sst>
 </file>
@@ -560,14 +557,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -943,477 +938,438 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4427E512-9369-2141-9D9A-2841123E1C13}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="34.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.796875" style="1"/>
+    <col min="5" max="5" width="11.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.6279272002381003E-4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9.0688388064708605E-5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.5918490081238602E-5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9.4244434287044505E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
-        <v>2.6279272002381003E-4</v>
-      </c>
-      <c r="D2" s="2">
-        <v>9.0688388064708605E-5</v>
-      </c>
-      <c r="E2" s="3">
-        <v>3.5918490081238602E-5</v>
-      </c>
-      <c r="F2" s="2">
-        <v>9.4244434287044505E-6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="1">
+        <v>1.04923251265238E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.0063859947693196E-4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.0299376353193998E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.7320387641818205E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.0215213048002799E-4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.97794604724473E-5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.28868497692047E-5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.0020587817516398E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>2.6279272002381003E-4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>9.0688388064708605E-5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>3.5918490081238602E-5</v>
-      </c>
-      <c r="F3" s="2">
-        <v>9.4244434287044505E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C5" s="1">
+        <v>2.2036345358525199E-4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.73650764956257E-5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.0598817493697899E-5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.0824397767754207E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.7091682578550102E-6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.6987277200806901E-6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.44207885667957E-6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.0688206525651099E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2">
-        <v>1.04923251265238E-3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8.0063859947693196E-4</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3.0299376353193998E-4</v>
-      </c>
-      <c r="F4" s="2">
-        <v>9.7320387641818205E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.0215213048002799E-4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5.97794604724473E-5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>2.28868497692047E-5</v>
-      </c>
-      <c r="F5" s="2">
-        <v>7.0020587817516398E-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="C8" s="1">
+        <v>8.4189765739352697E-7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.7086879338393499E-7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.80680878736269E-7</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5.47420884687663E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2">
-        <v>2.2036345358525199E-4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>7.73650764956257E-5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.0598817493697899E-5</v>
-      </c>
-      <c r="F6" s="2">
-        <v>8.0824397767754207E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.42192109488816E-5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5.9375518617808097E-6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.3183551127601798E-6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.5026027795722902E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2">
-        <v>8.7091682578550102E-6</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3.6987277200806901E-6</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.44207885667957E-6</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4.0688206525651099E-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2">
-        <v>8.4189765739352697E-7</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4.7086879338393499E-7</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.80680878736269E-7</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5.47420884687663E-8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C12">
+        <v>3.5195335169383303E-4</v>
+      </c>
+      <c r="D12">
+        <v>1.2127407176063527E-4</v>
+      </c>
+      <c r="E12">
+        <v>4.8038336725966984E-5</v>
+      </c>
+      <c r="F12">
+        <v>1.2597034452404395E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>1.5230145982138813E-3</v>
+      </c>
+      <c r="D13">
+        <v>1.156793267949673E-3</v>
+      </c>
+      <c r="E13">
+        <v>4.3785527215137318E-4</v>
+      </c>
+      <c r="F13">
+        <v>1.4053394633297537E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C14">
+        <v>4.9544002437275564E-4</v>
+      </c>
+      <c r="D14">
+        <v>2.9019956562906224E-4</v>
+      </c>
+      <c r="E14">
+        <v>1.1109918630241409E-4</v>
+      </c>
+      <c r="F14">
+        <v>3.3996603555700465E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1.0196696972986801E-3</v>
+      </c>
+      <c r="D15">
+        <v>3.58022611908352E-4</v>
+      </c>
+      <c r="E15">
+        <v>1.4160105037048387E-4</v>
+      </c>
+      <c r="F15">
+        <v>3.740432319130189E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2">
-        <v>1.42192109488816E-5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5.9375518617808097E-6</v>
-      </c>
-      <c r="E11" s="3">
-        <v>2.3183551127601798E-6</v>
-      </c>
-      <c r="F11" s="2">
-        <v>6.5026027795722902E-7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="C16">
+        <v>1.6436208313349941E-5</v>
+      </c>
+      <c r="D16">
+        <v>6.994579338644909E-6</v>
+      </c>
+      <c r="E16">
+        <v>2.7267038664696505E-6</v>
+      </c>
+      <c r="F16">
+        <v>7.6981973978587913E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>2.4140207869085528E-4</v>
+      </c>
+      <c r="D17">
+        <v>9.5827886140746653E-5</v>
+      </c>
+      <c r="E17">
+        <v>3.755011602571988E-5</v>
+      </c>
+      <c r="F17">
+        <v>1.036197317203149E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>8.9059604629766839E-7</v>
+      </c>
+      <c r="D18">
+        <v>4.3432315324689352E-7</v>
+      </c>
+      <c r="E18">
+        <v>1.6792766743283535E-7</v>
+      </c>
+      <c r="F18">
+        <v>4.9225260127496864E-8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>2.6606469426638246E-6</v>
+      </c>
+      <c r="D19">
+        <v>1.2193589120407524E-6</v>
+      </c>
+      <c r="E19">
+        <v>4.7323245509502039E-7</v>
+      </c>
+      <c r="F19">
+        <v>1.3641987108210757E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4">
-        <v>3.5195335169383303E-4</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.2127407176063527E-4</v>
-      </c>
-      <c r="E13" s="4">
-        <v>4.8038336725966984E-5</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1.2597034452404395E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3.5195335169383303E-4</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1.2127407176063527E-4</v>
-      </c>
-      <c r="E14" s="4">
-        <v>4.8038336725966984E-5</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1.2597034452404395E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1.5230145982138813E-3</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1.156793267949673E-3</v>
-      </c>
-      <c r="E15" s="4">
-        <v>4.3785527215137318E-4</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1.4053394633297537E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4.9544002437275564E-4</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2.9019956562906224E-4</v>
-      </c>
-      <c r="E16" s="4">
-        <v>1.1109918630241409E-4</v>
-      </c>
-      <c r="F16" s="4">
-        <v>3.3996603555700465E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="4">
-        <v>1.0196696972986801E-3</v>
-      </c>
-      <c r="D17" s="4">
-        <v>3.58022611908352E-4</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1.4160105037048387E-4</v>
-      </c>
-      <c r="F17" s="4">
-        <v>3.740432319130189E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="C20">
+        <v>1.7083200462685868E-6</v>
+      </c>
+      <c r="D20">
+        <v>8.6419400153336984E-7</v>
+      </c>
+      <c r="E20">
+        <v>3.3339878160241246E-7</v>
+      </c>
+      <c r="F20">
+        <v>9.8663431875040955E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="4">
-        <v>1.6436208313349941E-5</v>
-      </c>
-      <c r="D18" s="4">
-        <v>6.994579338644909E-6</v>
-      </c>
-      <c r="E18" s="4">
-        <v>2.7267038664696505E-6</v>
-      </c>
-      <c r="F18" s="4">
-        <v>7.6981973978587913E-7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2.4140207869085528E-4</v>
-      </c>
-      <c r="D19" s="4">
-        <v>9.5827886140746653E-5</v>
-      </c>
-      <c r="E19" s="4">
-        <v>3.755011602571988E-5</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1.036197317203149E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4">
-        <v>8.9059604629766839E-7</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4.3432315324689352E-7</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1.6792766743283535E-7</v>
-      </c>
-      <c r="F20" s="4">
-        <v>4.9225260127496864E-8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2.6606469426638246E-6</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1.2193589120407524E-6</v>
-      </c>
-      <c r="E21" s="4">
-        <v>4.7323245509502039E-7</v>
-      </c>
-      <c r="F21" s="4">
-        <v>1.3641987108210757E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1.7083200462685868E-6</v>
-      </c>
-      <c r="D22" s="4">
-        <v>8.6419400153336984E-7</v>
-      </c>
-      <c r="E22" s="4">
-        <v>3.3339878160241246E-7</v>
-      </c>
-      <c r="F22" s="4">
-        <v>9.8663431875040955E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="C21">
         <v>7.3765926245526248E-6</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D21">
         <v>4.7438598640607269E-6</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E21">
         <v>1.8081120982136274E-6</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F21">
         <v>5.6376027502899087E-7</v>
       </c>
     </row>

</xml_diff>